<commit_message>
m52 rev1.3 BOM added
</commit_message>
<xml_diff>
--- a/m52 PnP/Rev1.2 documents/BOM-speeduino v0.4.3 compatible PCB for m52 rev1.2.xlsx
+++ b/m52 PnP/Rev1.2 documents/BOM-speeduino v0.4.3 compatible PCB for m52 rev1.2.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev1.2 documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemppain\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev1.2 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EDBC045D-AFA9-4607-8BBC-B6A8A5BC2391}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E803E2-4F5F-45C1-99C9-82866CF981BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16515" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -159,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="308">
   <si>
     <t>Value</t>
   </si>
@@ -707,9 +712,6 @@
     <t>C1,C3,C5,C7,C9,C13,C15</t>
   </si>
   <si>
-    <t>D15,D17</t>
-  </si>
-  <si>
     <t>R2,R4,R6,R8,R22,R41</t>
   </si>
   <si>
@@ -797,9 +799,6 @@
     <t>LED1,LED2,LED3,LED5,LED6,LED7</t>
   </si>
   <si>
-    <t>D9,D10,D11,D18</t>
-  </si>
-  <si>
     <t>R25,R27,R31</t>
   </si>
   <si>
@@ -807,9 +806,6 @@
   </si>
   <si>
     <t>2.5-Bar MAP sensor</t>
-  </si>
-  <si>
-    <t>R63</t>
   </si>
   <si>
     <t>7.5k</t>
@@ -1203,6 +1199,114 @@
   <si>
     <t>ULN2003A 1</t>
   </si>
+  <si>
+    <t>Hardware for the optional connector</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note! The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Blue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ones are optional components A/C circuit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note! The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Orange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ones are optional for second external connector</t>
+    </r>
+  </si>
+  <si>
+    <t>D1,D15,D17</t>
+  </si>
+  <si>
+    <r>
+      <t>D16,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>D19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D9,D10,D11,D18,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>D20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R63,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>R66</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R7,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>R67,R68</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1211,7 +1315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1304,6 +1408,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Liberation Sans"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1476,7 +1604,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1572,14 +1700,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1976,10 +2107,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X54"/>
+  <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2194,10 +2325,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>11</v>
@@ -2219,13 +2350,13 @@
         <v>138</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="O4" s="5">
         <v>0.66</v>
@@ -2431,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>80</v>
@@ -2510,10 +2641,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>17</v>
@@ -2589,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>113</v>
@@ -2668,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>91</v>
@@ -2775,14 +2906,14 @@
     <row r="12" spans="1:24" ht="16.5" thickBot="1">
       <c r="A12" s="18">
         <f>LEN(C12)-LEN(SUBSTITUTE(C12,",",""))+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="18">
         <f t="shared" ref="B12:B15" si="9">LEN(D12)-LEN(SUBSTITUTE(D12,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>74</v>
+        <v>304</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>74</v>
@@ -2823,16 +2954,16 @@
       </c>
       <c r="Q12" s="6">
         <f>O12*A12</f>
-        <v>0.34</v>
+        <v>0.68</v>
       </c>
       <c r="R12" s="6">
         <f t="shared" si="6"/>
-        <v>0.43</v>
+        <v>0.86</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,1N5919BGOS-ND</v>
+        <v>2,1N5919BGOS-ND</v>
       </c>
       <c r="U12" s="4" t="str">
         <f t="shared" si="3"/>
@@ -2840,28 +2971,28 @@
       </c>
       <c r="V12" t="str">
         <f>"Diode - " &amp;A12&amp;"x "&amp;E12</f>
-        <v>Diode - 1x 1N5919BG Zener</v>
+        <v>Diode - 2x 1N5919BG Zener</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="4"/>
-        <v>863-1N5919BRLG|1</v>
+        <v>863-1N5919BRLG|2</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="5"/>
-        <v>1N5919BG 1</v>
+        <v>1N5919BG 2</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="26.25" thickBot="1">
       <c r="A13" s="18">
         <f>LEN(C13)-LEN(SUBSTITUTE(C13,",",""))+1</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="18">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>182</v>
+        <v>303</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>180</v>
@@ -2902,16 +3033,16 @@
       </c>
       <c r="Q13" s="6">
         <f>O13*A13</f>
-        <v>0.78</v>
+        <v>1.17</v>
       </c>
       <c r="R13" s="6">
         <f t="shared" si="6"/>
-        <v>0.78</v>
+        <v>1.17</v>
       </c>
       <c r="S13" s="4"/>
       <c r="T13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>2,1N5818-TPCT-ND</v>
+        <v>3,1N5818-TPCT-ND</v>
       </c>
       <c r="U13" s="4" t="str">
         <f t="shared" si="3"/>
@@ -2919,15 +3050,15 @@
       </c>
       <c r="V13" t="str">
         <f t="shared" ref="V13:V15" si="10">"Diode - " &amp;A13&amp;"x "&amp;E13</f>
-        <v>Diode - 2x 1N5818-TP Schottky</v>
+        <v>Diode - 3x 1N5818-TP Schottky</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="4"/>
-        <v>833-1N5818-TP|2</v>
+        <v>833-1N5818-TP|3</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="5"/>
-        <v>1N5818-TP 2</v>
+        <v>1N5818-TP 3</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="16.5" thickBot="1">
@@ -2940,7 +3071,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>109</v>
@@ -2961,7 +3092,7 @@
         <v>139</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>85</v>
@@ -3008,14 +3139,14 @@
     <row r="15" spans="1:24" ht="26.25" thickBot="1">
       <c r="A15" s="18">
         <f>LEN(C15)-LEN(SUBSTITUTE(C15,",",""))+1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="18">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>212</v>
+        <v>305</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>108</v>
@@ -3056,16 +3187,16 @@
       </c>
       <c r="Q15" s="6">
         <f>O15*A15</f>
-        <v>0.44</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R15" s="6">
         <f t="shared" si="6"/>
-        <v>0.44</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S15" s="4"/>
       <c r="T15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>4,1N4004-TPMSCT-ND</v>
+        <v>5,1N4004-TPMSCT-ND</v>
       </c>
       <c r="U15" s="4" t="str">
         <f t="shared" si="3"/>
@@ -3073,15 +3204,15 @@
       </c>
       <c r="V15" t="str">
         <f t="shared" si="10"/>
-        <v>Diode - 4x 1N4004</v>
+        <v>Diode - 5x 1N4004</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="4"/>
-        <v>833-1N4004-TP|4</v>
+        <v>833-1N4004-TP|5</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="5"/>
-        <v>1N4004-TP 4</v>
+        <v>1N4004-TP 5</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="16.5" thickBot="1">
@@ -3275,13 +3406,13 @@
         <v>139</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>88</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O19" s="6">
         <v>0.56000000000000005</v>
@@ -3329,16 +3460,16 @@
         <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>82</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -3346,19 +3477,19 @@
         <v>1</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="M20" s="30" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="O20" s="6">
         <v>1</v>
@@ -3404,16 +3535,16 @@
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>82</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -3421,19 +3552,19 @@
         <v>1</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L21" s="27" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="O21" s="6">
         <v>0.38</v>
@@ -3479,16 +3610,16 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>82</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -3496,19 +3627,19 @@
         <v>1</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L22" s="27" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="M22" s="30" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="O22" s="6">
         <v>0.23</v>
@@ -3597,7 +3728,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>107</v>
@@ -3606,7 +3737,7 @@
         <v>97</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>65</v>
@@ -3622,10 +3753,10 @@
         <v>138</v>
       </c>
       <c r="L24" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="M24" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>164</v>
@@ -3676,19 +3807,19 @@
         <v>6</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>107</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3">
@@ -3701,13 +3832,13 @@
         <v>138</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="M25" s="29" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O25" s="6">
         <v>2.62</v>
@@ -3756,19 +3887,19 @@
         <v>6</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>107</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3">
@@ -3781,13 +3912,13 @@
         <v>138</v>
       </c>
       <c r="L26" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="M26" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="M26" s="30" t="s">
-        <v>236</v>
-      </c>
       <c r="N26" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="O26" s="6">
         <v>0.25</v>
@@ -3872,10 +4003,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>40</v>
@@ -3895,13 +4026,13 @@
         <v>138</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>43</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O28" s="5">
         <v>0.08</v>
@@ -3949,10 +4080,10 @@
         <v>13</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>44</v>
@@ -3972,13 +4103,13 @@
         <v>138</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>46</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O29" s="5">
         <v>0.06</v>
@@ -4026,10 +4157,10 @@
         <v>2</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E30" s="13">
         <v>680</v>
@@ -4047,7 +4178,7 @@
         <v>138</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>114</v>
@@ -4103,7 +4234,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>136</v>
@@ -4180,16 +4311,16 @@
         <v>5</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>51</v>
@@ -4205,13 +4336,13 @@
         <v>138</v>
       </c>
       <c r="L32" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>193</v>
       </c>
       <c r="O32" s="5">
         <v>0.14000000000000001</v>
@@ -4258,7 +4389,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>71</v>
+        <v>307</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>71</v>
@@ -4337,7 +4468,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>112</v>
@@ -4360,13 +4491,13 @@
         <v>138</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>57</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O34" s="5">
         <v>0.1</v>
@@ -4414,7 +4545,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>110</v>
@@ -4484,23 +4615,23 @@
     <row r="36" spans="1:24" ht="26.25" thickBot="1">
       <c r="A36" s="18">
         <f>LEN(C36)-LEN(SUBSTITUTE(C36,",",""))+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" s="18">
         <f>LEN(D36)-LEN(SUBSTITUTE(D36,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>216</v>
+        <v>306</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>110</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -4514,11 +4645,11 @@
         <v>138</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O36" s="5"/>
       <c r="P36" s="5">
@@ -4530,7 +4661,7 @@
       </c>
       <c r="R36" s="6">
         <f t="shared" ref="R36" si="46">P36*A36</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S36" s="4"/>
       <c r="T36" s="4" t="str">
@@ -4543,16 +4674,16 @@
       </c>
       <c r="V36" t="str">
         <f t="shared" ref="V36" si="49">"Resistor - " &amp; A36&amp;"x "&amp;E36</f>
-        <v>Resistor - 1x 7.5k</v>
+        <v>Resistor - 2x 7.5k</v>
       </c>
       <c r="W36" t="str">
         <f t="shared" ref="W36" si="50">IF(NOT(N36=""),N36&amp;"|"&amp;A36,"")</f>
         <v>603-MFR-25FBF52-7K5
-|1</v>
+|2</v>
       </c>
       <c r="X36" t="str">
         <f t="shared" ref="X36" si="51">L36&amp;" "&amp;A36</f>
-        <v>MFR-25FBF52-7K5 1</v>
+        <v>MFR-25FBF52-7K5 2</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="16.5" thickBot="1">
@@ -4678,19 +4809,19 @@
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3">
@@ -4703,13 +4834,13 @@
         <v>138</v>
       </c>
       <c r="L39" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="M39" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="M39" s="35" t="s">
-        <v>297</v>
-      </c>
       <c r="N39" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="O39" s="5">
         <v>0.59</v>
@@ -4725,19 +4856,19 @@
       </c>
       <c r="S39" s="4"/>
       <c r="T39" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="U39" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="V39" t="s">
+        <v>297</v>
+      </c>
+      <c r="W39" t="s">
+        <v>298</v>
+      </c>
+      <c r="X39" t="s">
         <v>299</v>
-      </c>
-      <c r="U39" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="V39" t="s">
-        <v>300</v>
-      </c>
-      <c r="W39" t="s">
-        <v>301</v>
-      </c>
-      <c r="X39" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:24" ht="26.25" thickBot="1">
@@ -4749,19 +4880,19 @@
         <v>1</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3">
@@ -4772,13 +4903,13 @@
       </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="M40" s="31" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="O40" s="6">
         <v>12.79</v>
@@ -4831,7 +4962,7 @@
         <v>79</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>78</v>
@@ -4901,7 +5032,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>111</v>
@@ -5084,7 +5215,7 @@
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="3"/>
@@ -5123,16 +5254,16 @@
         <v>1</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>144</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="13"/>
@@ -5140,19 +5271,19 @@
         <v>1</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="K46" s="25" t="s">
         <v>138</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="M46" s="13" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="O46" s="6">
         <v>0.55000000000000004</v>
@@ -5198,16 +5329,16 @@
         <v>1</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>144</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="13"/>
@@ -5215,19 +5346,19 @@
         <v>1</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K47" s="25" t="s">
         <v>138</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="M47" s="13" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="O47" s="6">
         <v>0.33</v>
@@ -5273,16 +5404,16 @@
         <v>1</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>144</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="13"/>
@@ -5290,19 +5421,19 @@
         <v>1</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K48" s="25" t="s">
         <v>138</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="O48" s="6">
         <v>0.16</v>
@@ -5340,52 +5471,260 @@
         <v>39-00-0078 6</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="16.5" customHeight="1" thickBot="1">
+    <row r="49" spans="1:24" ht="16.5" thickBot="1">
       <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="3"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="13"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="33" t="s">
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="13"/>
+      <c r="M49" s="13"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+    </row>
+    <row r="50" spans="1:24" ht="16.5" thickBot="1">
+      <c r="A50" s="16"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+    </row>
+    <row r="51" spans="1:24" ht="16.5" thickBot="1">
+      <c r="A51" s="18">
+        <v>1</v>
+      </c>
+      <c r="B51" s="26">
+        <v>1</v>
+      </c>
+      <c r="C51" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13">
+        <v>1</v>
+      </c>
+      <c r="J51" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="K51" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="M51" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="O51" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="P51" s="6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="Q51" s="6">
+        <f>O51*A51</f>
+        <v>0.33</v>
+      </c>
+      <c r="R51" s="6">
+        <f>P51*A51</f>
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4" t="str">
+        <f>IF(NOT(M51=""),A51&amp;","&amp;M51,"")</f>
+        <v>1,WM3702-ND</v>
+      </c>
+      <c r="U51" s="4" t="str">
+        <f>IF(NOT(M51=""),B51&amp;","&amp;M51,"")</f>
+        <v>1,WM3702-ND</v>
+      </c>
+      <c r="V51" t="str">
+        <f>A51&amp;"x "&amp;E51</f>
+        <v>1x 6-POS connector</v>
+      </c>
+      <c r="W51" t="str">
+        <f>IF(NOT(N51=""),N51&amp;"|"&amp;A51,"")</f>
+        <v>538-39-01-2060|1</v>
+      </c>
+      <c r="X51" t="str">
+        <f>L51&amp;" "&amp;A51</f>
+        <v>39-01-2060 1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" ht="16.5" thickBot="1">
+      <c r="A52" s="18">
+        <v>6</v>
+      </c>
+      <c r="B52" s="26">
+        <v>1</v>
+      </c>
+      <c r="C52" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13">
+        <v>1</v>
+      </c>
+      <c r="J52" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="K52" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="M52" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="O52" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="P52" s="6">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="Q52" s="6">
+        <f>O52*A52</f>
+        <v>0.96</v>
+      </c>
+      <c r="R52" s="6">
+        <f>P52*A52</f>
+        <v>1.0859999999999999</v>
+      </c>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4" t="str">
+        <f>IF(NOT(M52=""),A52&amp;","&amp;M52,"")</f>
+        <v>6,WM9154-ND</v>
+      </c>
+      <c r="U52" s="4" t="str">
+        <f>IF(NOT(M52=""),B52&amp;","&amp;M52,"")</f>
+        <v>1,WM9154-ND</v>
+      </c>
+      <c r="V52" t="str">
+        <f>A52&amp;"x "&amp;E52</f>
+        <v>6x Female pin</v>
+      </c>
+      <c r="W52" t="str">
+        <f>IF(NOT(N52=""),N52&amp;"|"&amp;A52,"")</f>
+        <v>538-39-00-0078|6</v>
+      </c>
+      <c r="X52" t="str">
+        <f>L52&amp;" "&amp;A52</f>
+        <v>39-00-0078 6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="M49" s="34"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="1" t="s">
+      <c r="M53" s="35"/>
+      <c r="N53" s="32"/>
+      <c r="O53" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="11">
+      <c r="P53" s="1"/>
+      <c r="Q53" s="11">
         <f>SUM(Q3:Q48)</f>
-        <v>102.63000000000001</v>
-      </c>
-      <c r="R49" s="11">
+        <v>103.47000000000001</v>
+      </c>
+      <c r="R53" s="11">
         <f>SUM(R3:R48)</f>
-        <v>122.35199999999999</v>
-      </c>
-      <c r="S49" s="10" t="s">
+        <v>123.38200000000001</v>
+      </c>
+      <c r="S53" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
-      <c r="C53" t="s">
-        <v>258</v>
+    <row r="57" spans="1:24">
+      <c r="C57" t="s">
+        <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
-      <c r="C54" t="s">
-        <v>260</v>
+    <row r="58" spans="1:24">
+      <c r="C58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24">
+      <c r="C59" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24">
+      <c r="C60" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L53:M53"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>

</xml_diff>